<commit_message>
seteo automatico de facility y de cliente
</commit_message>
<xml_diff>
--- a/public/uploads/templates/templateListaOrdenes.xlsx
+++ b/public/uploads/templates/templateListaOrdenes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t xml:space="preserve">Ubicación Inicio</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sucursal</t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
@@ -76,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -97,6 +101,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,7 +155,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -171,23 +176,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -197,14 +199,14 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -237,30 +239,33 @@
       <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>